<commit_message>
corrections made regarding titles
</commit_message>
<xml_diff>
--- a/MPP Chinese translation.xlsx
+++ b/MPP Chinese translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kailee\Documents\GitHub\mannerpathChinese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512E2E0C-4647-4D3A-8936-30F9AB231B68}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834ABCE0-ACDD-4F07-8A0B-388DA2F4DD3B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6950" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10017,8 +10017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6DFD1F-345F-4526-807E-6A916CCFBA00}">
   <dimension ref="A1:CA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H37" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45:K50"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>

</xml_diff>